<commit_message>
Change Labor parameters from measurement profile to ecrf
</commit_message>
<xml_diff>
--- a/src/main/groovy/projects/gecco/crf/GroovyGenerator/Laboratory Values/Values/values_Values.xlsx
+++ b/src/main/groovy/projects/gecco/crf/GroovyGenerator/Laboratory Values/Values/values_Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Macedo\IdeaProjects\kairos-fhir-dsl-mapping-example\src\main\groovy\projects\gecco\crf\GroovyGenerator\Laboratory Values\Values\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB50FEEA-E407-42D1-8347-84E18F118589}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16F1CBC-5384-4434-95C2-E870ABBDDE1A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="121">
   <si>
     <t>IdComplement</t>
   </si>
@@ -371,6 +371,21 @@
   </si>
   <si>
     <t>Hemoglobin</t>
+  </si>
+  <si>
+    <t>COV_GECCO_FIBRINOGEN</t>
+  </si>
+  <si>
+    <t>fibrinogen</t>
+  </si>
+  <si>
+    <t>16859-1</t>
+  </si>
+  <si>
+    <t>Fibrinogen [Presence] in Platelet poor plasma</t>
+  </si>
+  <si>
+    <t>Fibrinogen</t>
   </si>
 </sst>
 </file>
@@ -1672,7 +1687,7 @@
   <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2199,12 +2214,24 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="A22" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="2"/>

</xml_diff>